<commit_message>
update code in business logic by Vilas
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Tutorials\git day1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA705340-689B-4F6E-A0AB-8F425D0E6A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>cloumn1</t>
+  </si>
+  <si>
+    <t>column2</t>
+  </si>
+  <si>
+    <t>cloumn3</t>
+  </si>
+  <si>
+    <t>column4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +353,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DataCollection And Survey Done By Vilas
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Tutorials\git day1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA705340-689B-4F6E-A0AB-8F425D0E6A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3B51F2-47B8-4A0F-B2D8-64DB6B862319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>cloumn1</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>column4</t>
+  </si>
+  <si>
+    <t>column5</t>
   </si>
 </sst>
 </file>
@@ -354,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E3"/>
+  <dimension ref="B3:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -374,6 +377,9 @@
       </c>
       <c r="E3" t="s">
         <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>